<commit_message>
Commit thirteen - Robot 5 complete
</commit_message>
<xml_diff>
--- a/Bot5/Bot5/ScrapedInvoiceData.xlsx
+++ b/Bot5/Bot5/ScrapedInvoiceData.xlsx
@@ -1,60 +1,266 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="122211"/>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <x:si>
+    <x:t>Company Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Dynazzy
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">279
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2170
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 725,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Yakidoo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">609
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3031
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">650,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Jamia
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">97
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">5536
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">925,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Mydo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">570
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2223
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">675,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tagopia
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">907
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3441
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 825,00 
+</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-</styleSheet>
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="30">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="4">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,37 +549,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="12.332031" style="2" customWidth="1"/>
+    <x:col min="3" max="3" width="14.554688" style="2" customWidth="1"/>
+    <x:col min="4" max="4" width="16.332031" style="2" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="3" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="3" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B5" s="3" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C5" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D5" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="3" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B6" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C6" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D6" s="3" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>